<commit_message>
Added latest team status and note for spring boot dependency manager
</commit_message>
<xml_diff>
--- a/Teams Progress/AIML-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIML-Teams-withLeaders.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6384B332-8F7C-4892-A726-C366EB752CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4FD4C1-E63B-4C62-A0FF-D6210D219448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Team Progress" sheetId="16" r:id="rId1"/>
+    <sheet name="Team Progress" sheetId="16" state="hidden" r:id="rId1"/>
     <sheet name="Team_1" sheetId="1" r:id="rId2"/>
     <sheet name="Team_2" sheetId="2" r:id="rId3"/>
     <sheet name="Team_3" sheetId="3" r:id="rId4"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="294">
   <si>
     <t>Student ID</t>
   </si>
@@ -897,10 +897,25 @@
     <t>Good Job - For names check the Team  sheet</t>
   </si>
   <si>
-    <t>Team 11</t>
-  </si>
-  <si>
-    <t>Team 12</t>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Spring XML Configuration</t>
+  </si>
+  <si>
+    <t>Spring Annotation Configuration</t>
+  </si>
+  <si>
+    <t>Spring Java Based Configuration</t>
+  </si>
+  <si>
+    <t>Spring Web MVC Project</t>
+  </si>
+  <si>
+    <t>Spring Boot Web Project</t>
+  </si>
+  <si>
+    <t>Spring Boot Simple App</t>
   </si>
 </sst>
 </file>
@@ -982,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -991,8 +1006,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1310,7 +1328,7 @@
   <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1444,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,15 +1474,33 @@
     <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>162</v>
       </c>
@@ -1472,7 +1508,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>164</v>
       </c>
@@ -1480,7 +1516,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>166</v>
       </c>
@@ -1488,7 +1524,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>168</v>
       </c>
@@ -1496,7 +1532,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>170</v>
       </c>
@@ -1504,7 +1540,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>172</v>
       </c>
@@ -1512,7 +1548,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>174</v>
       </c>
@@ -1520,7 +1556,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>176</v>
       </c>
@@ -1528,7 +1564,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>178</v>
       </c>
@@ -1536,7 +1572,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>180</v>
       </c>
@@ -1551,10 +1587,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1563,15 +1599,33 @@
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>182</v>
       </c>
@@ -1579,7 +1633,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>184</v>
       </c>
@@ -1587,7 +1641,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>186</v>
       </c>
@@ -1595,7 +1649,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>188</v>
       </c>
@@ -1603,7 +1657,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>190</v>
       </c>
@@ -1611,7 +1665,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>192</v>
       </c>
@@ -1619,7 +1673,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>194</v>
       </c>
@@ -1627,7 +1681,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>196</v>
       </c>
@@ -1635,7 +1689,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>198</v>
       </c>
@@ -1643,7 +1697,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>200</v>
       </c>
@@ -1658,10 +1712,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1670,15 +1724,33 @@
     <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>202</v>
       </c>
@@ -1686,7 +1758,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>204</v>
       </c>
@@ -1694,7 +1766,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>206</v>
       </c>
@@ -1702,7 +1774,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>208</v>
       </c>
@@ -1710,7 +1782,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>210</v>
       </c>
@@ -1718,7 +1790,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>212</v>
       </c>
@@ -1726,7 +1798,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>214</v>
       </c>
@@ -1734,7 +1806,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>216</v>
       </c>
@@ -1742,7 +1814,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>218</v>
       </c>
@@ -1750,12 +1822,20 @@
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -1765,10 +1845,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1777,15 +1857,33 @@
     <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>222</v>
       </c>
@@ -1793,7 +1891,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>224</v>
       </c>
@@ -1801,7 +1899,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>226</v>
       </c>
@@ -1809,7 +1907,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>228</v>
       </c>
@@ -1817,7 +1915,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>230</v>
       </c>
@@ -1825,7 +1923,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>232</v>
       </c>
@@ -1833,7 +1931,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>234</v>
       </c>
@@ -1841,7 +1939,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>236</v>
       </c>
@@ -1849,7 +1947,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>238</v>
       </c>
@@ -1857,12 +1955,20 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>240</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1872,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1884,15 +1990,33 @@
     <col min="2" max="2" width="25.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>242</v>
       </c>
@@ -1900,7 +2024,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>244</v>
       </c>
@@ -1908,7 +2032,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>246</v>
       </c>
@@ -1916,7 +2040,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>248</v>
       </c>
@@ -1924,7 +2048,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>250</v>
       </c>
@@ -1932,7 +2056,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>252</v>
       </c>
@@ -1940,7 +2064,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>254</v>
       </c>
@@ -1948,7 +2072,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>256</v>
       </c>
@@ -1956,7 +2080,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>258</v>
       </c>
@@ -1964,7 +2088,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>260</v>
       </c>
@@ -1979,10 +2103,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2006,38 +2130,8 @@
       <c r="B2" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C2" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C5" t="s">
-        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2047,10 +2141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2060,27 +2154,47 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8">
-        <v>45839</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="8"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2088,8 +2202,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2097,8 +2216,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2106,8 +2230,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2115,17 +2244,27 @@
         <v>11</v>
       </c>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="8"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2133,8 +2272,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -2142,8 +2286,13 @@
         <v>17</v>
       </c>
       <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -2151,8 +2300,13 @@
         <v>19</v>
       </c>
       <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2160,6 +2314,25 @@
         <v>21</v>
       </c>
       <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2168,10 +2341,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2180,15 +2353,33 @@
     <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2196,7 +2387,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -2204,7 +2395,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -2212,7 +2403,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -2220,7 +2411,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -2228,7 +2419,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -2236,7 +2427,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -2244,7 +2435,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -2252,7 +2443,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
@@ -2260,7 +2451,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -2275,10 +2466,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2287,15 +2478,33 @@
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -2303,7 +2512,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
@@ -2311,7 +2520,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
@@ -2320,7 +2529,7 @@
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
@@ -2328,7 +2537,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -2337,7 +2546,7 @@
       </c>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -2346,7 +2555,7 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -2354,7 +2563,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -2362,7 +2571,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
@@ -2371,7 +2580,7 @@
       </c>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>60</v>
       </c>
@@ -2386,10 +2595,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2398,15 +2607,33 @@
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
@@ -2414,7 +2641,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>64</v>
       </c>
@@ -2422,7 +2649,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
@@ -2430,7 +2657,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>68</v>
       </c>
@@ -2438,7 +2665,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
@@ -2446,7 +2673,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>72</v>
       </c>
@@ -2454,7 +2681,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
@@ -2462,7 +2689,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>76</v>
       </c>
@@ -2470,7 +2697,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>78</v>
       </c>
@@ -2478,7 +2705,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>80</v>
       </c>
@@ -2493,10 +2720,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2506,106 +2733,121 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8">
-        <v>45839</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2614,10 +2856,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2627,106 +2869,121 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8">
-        <v>45839</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2735,10 +2992,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2747,15 +3004,33 @@
     <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>122</v>
       </c>
@@ -2763,7 +3038,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
@@ -2771,7 +3046,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>126</v>
       </c>
@@ -2779,7 +3054,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>128</v>
       </c>
@@ -2787,7 +3062,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>130</v>
       </c>
@@ -2795,7 +3070,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>132</v>
       </c>
@@ -2803,7 +3078,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>134</v>
       </c>
@@ -2811,7 +3086,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>136</v>
       </c>
@@ -2819,7 +3094,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>138</v>
       </c>
@@ -2827,7 +3102,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>140</v>
       </c>
@@ -2842,10 +3117,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2854,15 +3129,33 @@
     <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>142</v>
       </c>
@@ -2870,7 +3163,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>144</v>
       </c>
@@ -2878,7 +3171,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>146</v>
       </c>
@@ -2886,7 +3179,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>148</v>
       </c>
@@ -2894,7 +3187,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>150</v>
       </c>
@@ -2902,7 +3195,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
@@ -2910,7 +3203,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>154</v>
       </c>
@@ -2918,7 +3211,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>156</v>
       </c>
@@ -2926,7 +3219,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>158</v>
       </c>
@@ -2934,7 +3227,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
Reformated multi threading, maven & updated team progress
</commit_message>
<xml_diff>
--- a/Teams Progress/AIML-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIML-Teams-withLeaders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3093FF-72DF-4B0F-84F1-C2E4FEADC45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50821888-5FB2-4E11-BA0B-8FAE024F89A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Team Progress" sheetId="16" state="hidden" r:id="rId1"/>
     <sheet name="Team_1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Team_1!$A$1:$K$135</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1004,7 +1007,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1034,8 +1037,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1058,22 +1067,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1081,15 +1079,12 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1543,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="I129" sqref="I129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1561,31 +1556,31 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="8" t="s">
         <v>302</v>
       </c>
     </row>
@@ -1596,16 +1591,17 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="7"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1614,7 +1610,7 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D3" s="2"/>
@@ -1623,6 +1619,8 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1631,7 +1629,7 @@
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D4" s="2"/>
@@ -1641,6 +1639,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="7"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1649,7 +1648,7 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D5" s="2"/>
@@ -1658,6 +1657,8 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1666,7 +1667,7 @@
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D6" s="2"/>
@@ -1675,6 +1676,8 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1683,16 +1686,17 @@
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="7"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1701,7 +1705,7 @@
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D8" s="2"/>
@@ -1710,6 +1714,8 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1718,7 +1724,7 @@
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D9" s="2"/>
@@ -1727,15 +1733,17 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D10" s="2"/>
@@ -1744,6 +1752,8 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1752,7 +1762,7 @@
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D11" s="2"/>
@@ -1761,6 +1771,8 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1769,7 +1781,7 @@
       <c r="B12" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D12" s="2"/>
@@ -1779,6 +1791,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="7"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1787,26 +1800,40 @@
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="J13" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="s">
         <v>294</v>
       </c>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="J14" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
         <v>294</v>
       </c>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -1815,9 +1842,17 @@
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>305</v>
       </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -1826,1480 +1861,2353 @@
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>306</v>
       </c>
       <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>306</v>
       </c>
       <c r="D27" s="7"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
       <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>306</v>
       </c>
       <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>306</v>
       </c>
       <c r="D31" s="7"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
       <c r="J31" s="7"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>307</v>
       </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
       <c r="J34" s="7"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>307</v>
       </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
       <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>307</v>
       </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
       <c r="J42" s="7" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F44" s="8"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
       <c r="J44" s="7"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K44" s="7"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
       <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
       <c r="J49" s="7"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="D53" s="2"/>
       <c r="E53" s="2"/>
-      <c r="J53" s="8"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-      <c r="J54" s="8"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="D55" s="2"/>
       <c r="E55" s="2"/>
-      <c r="J55" s="8"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="J56" s="8"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E57" s="8"/>
-      <c r="J57" s="8"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D57" s="2"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="J58" t="s">
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="J59" s="8"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="2"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E60" s="8"/>
-      <c r="J60" t="s">
+      <c r="D60" s="2"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K60" s="2"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-      <c r="J61" s="8"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="2"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-      <c r="J62" s="8"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="2"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J63" t="s">
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K63" s="2"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J64" t="s">
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K64" s="2"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J65" t="s">
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K65" s="2"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J66" t="s">
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K66" s="2"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J67" t="s">
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K67" s="2"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J68" t="s">
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K68" s="2"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J69" t="s">
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K69" s="2"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J70" t="s">
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K70" s="2"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J71" t="s">
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K71" s="2"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J72" t="s">
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K72" s="2"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J73" t="s">
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K73" s="2"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J74" t="s">
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K74" s="2"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J75" t="s">
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K75" s="2"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J76" t="s">
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K76" s="2"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J77" t="s">
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K77" s="2"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J78" t="s">
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K78" s="2"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J79" t="s">
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K79" s="2"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J80" t="s">
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K80" s="2"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J81" t="s">
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K81" s="2"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="J83" t="s">
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K83" s="2"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>164</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="2" t="s">
         <v>312</v>
       </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
       <c r="J86" s="7" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K86" s="2"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
+      <c r="K88" s="2"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
       <c r="J93" s="7"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K93" s="2"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
       <c r="J94" s="7"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K94" s="2"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B95" s="11" t="s">
+      <c r="B95" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
       <c r="J95" s="7"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K95" s="7"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
       <c r="J96" s="7"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K96" s="2"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
       <c r="J97" s="7"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K97" s="2"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
       <c r="J98" s="7"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K98" s="2"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>194</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
       <c r="J99" s="7"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K99" s="2"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
       <c r="J100" s="7"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K100" s="2"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
       <c r="J101" s="7"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K101" s="2"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>200</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
       <c r="J102" s="7"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K102" s="2"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="2" t="s">
         <v>314</v>
       </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
       <c r="J103" s="7"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K103" s="2"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B107" s="11" t="s">
+      <c r="B107" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="2" t="s">
         <v>314</v>
       </c>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
       <c r="J107" s="7"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K107" s="2"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="J109" t="s">
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K109" s="2"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="2" t="s">
         <v>314</v>
       </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
       <c r="J112" s="7"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K112" s="2"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>266</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>222</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>224</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>226</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>228</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>230</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>232</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+      <c r="J119" s="2"/>
+      <c r="K119" s="2"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>234</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="B121" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="2" t="s">
         <v>315</v>
       </c>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
       <c r="J121" s="7"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K121" s="2"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>238</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>240</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="J123" t="s">
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K123" s="2"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J125" t="s">
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K125" s="2"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>244</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J126" t="s">
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+      <c r="J126" s="2" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K126" s="2"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>246</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J127" t="s">
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+      <c r="J127" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K127" s="2"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B128" s="11" t="s">
+      <c r="B128" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J128" t="s">
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+      <c r="J128" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K128" s="2"/>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>250</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J129" t="s">
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+      <c r="H129" s="2"/>
+      <c r="I129" s="2"/>
+      <c r="J129" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K129" s="2"/>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>252</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J130" t="s">
+      <c r="D130" s="2"/>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
+      <c r="J130" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K130" s="2"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>254</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J131" t="s">
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+      <c r="H131" s="2"/>
+      <c r="I131" s="2"/>
+      <c r="J131" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K131" s="2"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J132" t="s">
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+      <c r="H132" s="2"/>
+      <c r="I132" s="2"/>
+      <c r="J132" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K132" s="2"/>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J133" t="s">
+      <c r="D133" s="2"/>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+      <c r="J133" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K133" s="2"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>260</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J134" t="s">
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+      <c r="J134" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K134" s="2"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>262</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="2" t="s">
         <v>317</v>
       </c>
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+      <c r="H135" s="2"/>
+      <c r="I135" s="2"/>
+      <c r="J135" s="2"/>
+      <c r="K135" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K135" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated team progress and added content for week 6 day 1
</commit_message>
<xml_diff>
--- a/Teams Progress/AIML-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIML-Teams-withLeaders.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B20670-0A73-4698-B82A-EF28ECF065A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716740C5-6EEB-4ED1-9347-BEDFF0BE28BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Progress" sheetId="16" state="hidden" r:id="rId1"/>
     <sheet name="Team_1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Team_1!$A$1:$K$135</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="320">
   <si>
     <t>Student ID</t>
   </si>
@@ -978,6 +979,12 @@
   </si>
   <si>
     <t>????</t>
+  </si>
+  <si>
+    <t>internship</t>
+  </si>
+  <si>
+    <t>absent</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1091,8 +1098,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1544,10 +1552,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1592,7 +1601,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1609,9 +1618,9 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1628,13 +1637,13 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1647,9 +1656,9 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1666,9 +1675,9 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1685,9 +1694,9 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1704,9 +1713,9 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1723,9 +1732,9 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1742,13 +1751,13 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1761,9 +1770,9 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1780,9 +1789,9 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>264</v>
       </c>
@@ -1799,17 +1808,17 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1817,20 +1826,18 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J13" s="2"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1838,39 +1845,37 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J14" s="2"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>306</v>
+      </c>
+      <c r="D15" s="7"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1879,55 +1884,55 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>306</v>
+      </c>
+      <c r="D17" s="7"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>306</v>
+      </c>
+      <c r="D18" s="7"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1936,17 +1941,17 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1955,36 +1960,36 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>306</v>
+      </c>
+      <c r="D21" s="7"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>41</v>
+        <v>60</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1993,17 +1998,17 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2012,17 +2017,17 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2033,17 +2038,17 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>47</v>
+        <v>68</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D25" s="7"/>
+        <v>307</v>
+      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2052,15 +2057,15 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2071,53 +2076,53 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D27" s="7"/>
+        <v>307</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="7"/>
+      <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>78</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D28" s="7"/>
+        <v>307</v>
+      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>80</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2125,18 +2130,20 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J29" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2145,36 +2152,36 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>59</v>
+        <v>86</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D31" s="7"/>
+        <v>308</v>
+      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J31" s="2"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -2183,17 +2190,17 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -2202,17 +2209,17 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2220,18 +2227,18 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="7"/>
+      <c r="J34" s="2"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2239,18 +2246,18 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2259,17 +2266,17 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2277,18 +2284,20 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J37" s="2"/>
+      <c r="K37" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2297,17 +2306,19 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K38" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2315,18 +2326,18 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2334,18 +2345,18 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>79</v>
+        <v>106</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2353,18 +2364,18 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>81</v>
+        <v>108</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2372,58 +2383,58 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="J42" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>83</v>
+        <v>110</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="E43" s="7"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>85</v>
+        <v>112</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="7"/>
+      <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J44" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="K44" s="9"/>
+    </row>
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>87</v>
+        <v>114</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2431,37 +2442,39 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>89</v>
+        <v>116</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
+      <c r="E46" s="7"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J46" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="K46" s="9"/>
+    </row>
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2469,18 +2482,18 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+    </row>
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -2488,18 +2501,18 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>95</v>
+        <v>162</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2507,18 +2520,22 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J49" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>96</v>
+        <v>164</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>97</v>
+        <v>165</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2527,17 +2544,19 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K50" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>98</v>
+        <v>166</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2546,17 +2565,19 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K51" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>101</v>
+        <v>169</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -2564,18 +2585,20 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J52" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="K52" s="7"/>
+    </row>
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>103</v>
+        <v>170</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -2583,18 +2606,18 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J53" s="2"/>
+      <c r="K53" s="7"/>
+    </row>
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>105</v>
+        <v>173</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2602,18 +2625,20 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="2"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J54" s="2"/>
+      <c r="K54" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>106</v>
+        <v>174</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2621,18 +2646,18 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="2"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J55" s="2"/>
+      <c r="K55" s="7"/>
+    </row>
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2640,37 +2665,39 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="2"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J56" s="2"/>
+      <c r="K56" s="7"/>
+    </row>
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>111</v>
+        <v>178</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D57" s="2"/>
-      <c r="E57" s="7"/>
+      <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="2"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J57" s="2"/>
+      <c r="K57" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -2678,20 +2705,18 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
-      <c r="J58" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="K58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="7"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>114</v>
+        <v>182</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
+        <v>183</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -2700,38 +2725,36 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="7"/>
-      <c r="K59" s="2"/>
+      <c r="K59" s="7"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>117</v>
+        <v>184</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D60" s="2"/>
-      <c r="E60" s="7"/>
+      <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
-      <c r="J60" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="K60" s="2"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>118</v>
+        <v>188</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>119</v>
+        <v>189</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -2740,17 +2763,17 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="7"/>
-      <c r="K61" s="2"/>
+      <c r="K61" s="7"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>121</v>
+        <v>191</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -2759,17 +2782,17 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="7"/>
-      <c r="K62" s="2"/>
+      <c r="K62" s="7"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>123</v>
+        <v>192</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -2777,20 +2800,18 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
-      <c r="J63" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K63" s="2"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>124</v>
+        <v>194</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>125</v>
+        <v>195</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -2798,20 +2819,18 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
-      <c r="J64" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K64" s="2"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>127</v>
+        <v>196</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -2819,20 +2838,18 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K65" s="2"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>129</v>
+        <v>198</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -2840,20 +2857,18 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
-      <c r="J66" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K66" s="2"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -2861,20 +2876,18 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
-      <c r="J67" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K67" s="2"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J67" s="7"/>
+      <c r="K67" s="12"/>
+    </row>
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>133</v>
+        <v>202</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -2882,20 +2895,18 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
-      <c r="J68" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K68" s="2"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J68" s="7"/>
+      <c r="K68" s="9"/>
+    </row>
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>135</v>
+        <v>205</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -2903,20 +2914,18 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
-      <c r="J69" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K69" s="2"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J69" s="2"/>
+      <c r="K69" s="9"/>
+    </row>
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>136</v>
+        <v>206</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>137</v>
+        <v>207</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -2924,20 +2933,18 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
-      <c r="J70" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K70" s="2"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J70" s="2"/>
+      <c r="K70" s="9"/>
+    </row>
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>138</v>
+        <v>208</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>139</v>
+        <v>209</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -2945,20 +2952,18 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
-      <c r="J71" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K71" s="2"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J71" s="2"/>
+      <c r="K71" s="9"/>
+    </row>
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>140</v>
+        <v>210</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>141</v>
+        <v>211</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -2966,20 +2971,18 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
-      <c r="J72" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K72" s="2"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+    </row>
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>142</v>
+        <v>212</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>143</v>
+        <v>213</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -2987,20 +2990,18 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
-      <c r="J73" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K73" s="2"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J73" s="2"/>
+      <c r="K73" s="9"/>
+    </row>
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>144</v>
+        <v>214</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -3009,19 +3010,19 @@
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K74" s="2"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+      <c r="K74" s="9"/>
+    </row>
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>147</v>
+        <v>216</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -3029,20 +3030,18 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
-      <c r="J75" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K75" s="2"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J75" s="2"/>
+      <c r="K75" s="9"/>
+    </row>
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>148</v>
+        <v>218</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>149</v>
+        <v>219</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -3050,20 +3049,18 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
-      <c r="J76" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K76" s="2"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J76" s="2"/>
+      <c r="K76" s="9"/>
+    </row>
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>151</v>
+        <v>221</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -3071,20 +3068,18 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
-      <c r="J77" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K77" s="2"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J77" s="7"/>
+      <c r="K77" s="9"/>
+    </row>
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>153</v>
+        <v>266</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -3092,20 +3087,18 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
-      <c r="J78" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="9"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>155</v>
+        <v>262</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -3113,20 +3106,18 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
-      <c r="J79" s="2" t="s">
-        <v>298</v>
-      </c>
+      <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>156</v>
+        <v>22</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -3135,19 +3126,19 @@
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K80" s="2"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+      <c r="K80" s="9"/>
+    </row>
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>159</v>
+        <v>24</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -3156,19 +3147,19 @@
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K81" s="2"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+      <c r="K81" s="9"/>
+    </row>
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>160</v>
+        <v>26</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>161</v>
+        <v>27</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -3177,17 +3168,17 @@
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K82" s="9"/>
+    </row>
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B83" s="11" t="s">
-        <v>163</v>
+        <v>28</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -3195,20 +3186,18 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
-      <c r="J83" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="K83" s="2"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J83" s="2"/>
+      <c r="K83" s="9"/>
+    </row>
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>165</v>
+        <v>31</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -3217,17 +3206,17 @@
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K84" s="9"/>
+    </row>
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>167</v>
+        <v>33</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -3236,17 +3225,17 @@
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K85" s="9"/>
+    </row>
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>168</v>
+        <v>34</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>169</v>
+        <v>35</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -3254,20 +3243,18 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
-      <c r="J86" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="K86" s="2"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J86" s="2"/>
+      <c r="K86" s="9"/>
+    </row>
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>171</v>
+        <v>36</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -3276,17 +3263,17 @@
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K87" s="9"/>
+    </row>
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>172</v>
+        <v>38</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>173</v>
+        <v>39</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -3295,17 +3282,17 @@
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K88" s="9"/>
+    </row>
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>175</v>
+        <v>40</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -3314,17 +3301,17 @@
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K89" s="9"/>
+    </row>
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>176</v>
+        <v>64</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>177</v>
+        <v>65</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -3332,18 +3319,18 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+    </row>
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>179</v>
+        <v>70</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -3351,18 +3338,18 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
-      <c r="K91" s="2"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
+    </row>
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>180</v>
+        <v>74</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>181</v>
+        <v>75</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -3371,36 +3358,36 @@
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
-      <c r="K92" s="2"/>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K92" s="7"/>
+    </row>
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>183</v>
+        <v>84</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
+      <c r="F93" s="7"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
       <c r="J93" s="7"/>
-      <c r="K93" s="2"/>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K93" s="7"/>
+    </row>
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>184</v>
+        <v>122</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>185</v>
+        <v>123</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -3408,18 +3395,20 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="2"/>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J94" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K94" s="9"/>
+    </row>
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B95" s="11" t="s">
-        <v>187</v>
+        <v>124</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -3427,18 +3416,20 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
-      <c r="J95" s="7"/>
+      <c r="J95" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="K95" s="7"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>189</v>
+        <v>126</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>127</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -3446,18 +3437,20 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
-      <c r="J96" s="7"/>
-      <c r="K96" s="2"/>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J96" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K96" s="7"/>
+    </row>
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>191</v>
+        <v>128</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -3465,18 +3458,20 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
-      <c r="J97" s="7"/>
-      <c r="K97" s="2"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J97" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K97" s="7"/>
+    </row>
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>193</v>
+        <v>130</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -3484,18 +3479,20 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
-      <c r="J98" s="7"/>
-      <c r="K98" s="2"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J98" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K98" s="9"/>
+    </row>
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>194</v>
+        <v>132</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>195</v>
+        <v>133</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -3503,18 +3500,20 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
-      <c r="J99" s="7"/>
-      <c r="K99" s="2"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J99" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K99" s="7"/>
+    </row>
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -3522,18 +3521,20 @@
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
-      <c r="J100" s="7"/>
-      <c r="K100" s="2"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J100" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K100" s="9"/>
+    </row>
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>198</v>
+        <v>136</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>199</v>
+        <v>137</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -3541,18 +3542,20 @@
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
-      <c r="J101" s="7"/>
-      <c r="K101" s="2"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J101" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K101" s="7"/>
+    </row>
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>200</v>
+        <v>138</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>201</v>
+        <v>139</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -3560,18 +3563,20 @@
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
-      <c r="J102" s="7"/>
-      <c r="K102" s="2"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J102" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K102" s="7"/>
+    </row>
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>203</v>
+        <v>140</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -3579,18 +3584,20 @@
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
-      <c r="J103" s="7"/>
-      <c r="K103" s="2"/>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J103" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K103" s="9"/>
+    </row>
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B104" s="11" t="s">
-        <v>205</v>
+        <v>142</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -3598,18 +3605,20 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J104" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K104" s="9"/>
+    </row>
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>207</v>
+        <v>145</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -3617,18 +3626,20 @@
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
-      <c r="K105" s="2"/>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J105" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K105" s="9"/>
+    </row>
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>209</v>
+        <v>146</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>147</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
@@ -3636,18 +3647,20 @@
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
-      <c r="K106" s="2"/>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J106" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K106" s="9"/>
+    </row>
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B107" s="10" t="s">
-        <v>211</v>
+        <v>148</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
@@ -3655,18 +3668,20 @@
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
-      <c r="J107" s="7"/>
-      <c r="K107" s="2"/>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J107" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K107" s="9"/>
+    </row>
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>213</v>
+        <v>151</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
@@ -3674,18 +3689,20 @@
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J108" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K108" s="9"/>
+    </row>
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>215</v>
+        <v>152</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
@@ -3694,19 +3711,19 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="K109" s="2"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+      <c r="K109" s="9"/>
+    </row>
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>217</v>
+        <v>154</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
@@ -3714,18 +3731,20 @@
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J110" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K110" s="9"/>
+    </row>
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>218</v>
+        <v>156</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
@@ -3733,18 +3752,20 @@
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
-      <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J111" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K111" s="9"/>
+    </row>
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>220</v>
+        <v>158</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>221</v>
+        <v>159</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
@@ -3752,18 +3773,20 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
-      <c r="J112" s="7"/>
-      <c r="K112" s="2"/>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J112" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K112" s="9"/>
+    </row>
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>266</v>
+        <v>160</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>267</v>
+        <v>161</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
@@ -3772,17 +3795,17 @@
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
-      <c r="K113" s="2"/>
+      <c r="K113" s="9"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>223</v>
+        <v>186</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>187</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
@@ -3790,15 +3813,15 @@
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
-      <c r="J114" s="2"/>
-      <c r="K114" s="2"/>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J114" s="7"/>
+      <c r="K114" s="7"/>
+    </row>
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>315</v>
@@ -3810,14 +3833,14 @@
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
-      <c r="K115" s="2"/>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K115" s="7"/>
+    </row>
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>315</v>
@@ -3829,14 +3852,14 @@
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
-      <c r="K116" s="2"/>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K116" s="7"/>
+    </row>
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>315</v>
@@ -3848,14 +3871,14 @@
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
       <c r="J117" s="2"/>
-      <c r="K117" s="2"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K117" s="7"/>
+    </row>
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>315</v>
@@ -3867,14 +3890,14 @@
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
       <c r="J118" s="2"/>
-      <c r="K118" s="2"/>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K118" s="7"/>
+    </row>
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>315</v>
@@ -3886,14 +3909,14 @@
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
       <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K119" s="7"/>
+    </row>
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>315</v>
@@ -3905,14 +3928,14 @@
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
       <c r="J120" s="2"/>
-      <c r="K120" s="2"/>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K120" s="7"/>
+    </row>
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B121" s="11" t="s">
-        <v>237</v>
+        <v>234</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>315</v>
@@ -3923,15 +3946,15 @@
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
-      <c r="J121" s="7"/>
-      <c r="K121" s="2"/>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J121" s="2"/>
+      <c r="K121" s="7"/>
+    </row>
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>315</v>
@@ -3942,15 +3965,15 @@
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
-      <c r="J122" s="2"/>
-      <c r="K122" s="2"/>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J122" s="7"/>
+      <c r="K122" s="7"/>
+    </row>
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>315</v>
@@ -3961,17 +3984,15 @@
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
-      <c r="J123" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="K123" s="2"/>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J123" s="2"/>
+      <c r="K123" s="7"/>
+    </row>
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>269</v>
+        <v>240</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>315</v>
@@ -3982,18 +4003,20 @@
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
-      <c r="J124" s="2"/>
-      <c r="K124" s="2"/>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J124" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="K124" s="7"/>
+    </row>
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
@@ -4001,17 +4024,15 @@
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
-      <c r="J125" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="K125" s="2"/>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J125" s="2"/>
+      <c r="K125" s="7"/>
+    </row>
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>316</v>
@@ -4023,16 +4044,16 @@
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
       <c r="J126" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="K126" s="2"/>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+      <c r="K126" s="9"/>
+    </row>
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>316</v>
@@ -4044,16 +4065,16 @@
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
       <c r="J127" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="K127" s="2"/>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+      <c r="K127" s="7"/>
+    </row>
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B128" s="11" t="s">
-        <v>249</v>
+        <v>246</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>316</v>
@@ -4065,16 +4086,16 @@
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
       <c r="J128" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K128" s="2"/>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+      <c r="K128" s="9"/>
+    </row>
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
+      </c>
+      <c r="B129" s="10" t="s">
+        <v>249</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>316</v>
@@ -4086,16 +4107,16 @@
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
       <c r="J129" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="K129" s="2"/>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+      <c r="K129" s="9"/>
+    </row>
+    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>316</v>
@@ -4107,16 +4128,16 @@
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
       <c r="J130" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K130" s="2"/>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+      <c r="K130" s="9"/>
+    </row>
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>316</v>
@@ -4130,14 +4151,14 @@
       <c r="J131" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="K131" s="2"/>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K131" s="9"/>
+    </row>
+    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>316</v>
@@ -4149,16 +4170,16 @@
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
       <c r="J132" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="K132" s="2"/>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+      <c r="K132" s="9"/>
+    </row>
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>316</v>
@@ -4170,16 +4191,16 @@
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
       <c r="J133" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K133" s="2"/>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+      <c r="K133" s="9"/>
+    </row>
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>316</v>
@@ -4191,19 +4212,19 @@
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
       <c r="J134" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="K134" s="2"/>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+      <c r="K134" s="9"/>
+    </row>
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
@@ -4211,11 +4232,123 @@
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
-      <c r="J135" s="2"/>
-      <c r="K135" s="2"/>
+      <c r="J135" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="K135" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K135" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K135" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="????"/>
+        <filter val="Team_10"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CD5E78-C81B-4997-BD7D-58E393B821D0}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>13</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>9</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="12" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14" s="9" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>